<commit_message>
Updated global.R to incldue manually-added receipts. Updated ui to change order of grocery plots. Updated server.r to split category plots into current month vs average. Added more transactions data.
</commit_message>
<xml_diff>
--- a/SpendTracker_ShinyApp/pastTransactionsData/manuallyEnteredGroceryReceipts.xlsx
+++ b/SpendTracker_ShinyApp/pastTransactionsData/manuallyEnteredGroceryReceipts.xlsx
@@ -16,19 +16,160 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>asdfasdf</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>bread</t>
+  </si>
+  <si>
+    <t>Frozen peas</t>
+  </si>
+  <si>
+    <t>Bagels</t>
+  </si>
+  <si>
+    <t>Potatoes</t>
+  </si>
+  <si>
+    <t>Cream cheese</t>
+  </si>
+  <si>
+    <t>Cherry tomatoes</t>
+  </si>
+  <si>
+    <t>Fresh produce courgette</t>
+  </si>
+  <si>
+    <t>Fresh produce kumara</t>
+  </si>
+  <si>
+    <t>Pasta</t>
+  </si>
+  <si>
+    <t>Cadbury flake</t>
+  </si>
+  <si>
+    <t>Nestlé milky bar</t>
+  </si>
+  <si>
+    <t>Black Knight liquorice</t>
+  </si>
+  <si>
+    <t>Only organic cake</t>
+  </si>
+  <si>
+    <t>Watties potato and leek soup</t>
+  </si>
+  <si>
+    <t>Kleenex tissues</t>
+  </si>
+  <si>
+    <t>saline nasal spray</t>
+  </si>
+  <si>
+    <t>McIntosh toffees</t>
+  </si>
+  <si>
+    <t>Red lentils</t>
+  </si>
+  <si>
+    <t>Chicken thighs</t>
+  </si>
+  <si>
+    <t>Beef mince</t>
+  </si>
+  <si>
+    <t>Maltesers</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>Anchor dairy blend</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>dried apricots</t>
+  </si>
+  <si>
+    <t>nappies</t>
+  </si>
+  <si>
+    <t>tampons</t>
+  </si>
+  <si>
+    <t>Raffertys organic banana porridge</t>
+  </si>
+  <si>
+    <t>nurofen</t>
+  </si>
+  <si>
+    <t>olive oil</t>
+  </si>
+  <si>
+    <t>milk</t>
+  </si>
+  <si>
+    <t>marmalade</t>
+  </si>
+  <si>
+    <t>fresh produce potatoes</t>
+  </si>
+  <si>
+    <t>only organic vege lasagne</t>
+  </si>
+  <si>
+    <t>fresh produce bananas</t>
+  </si>
+  <si>
+    <t>chocolate</t>
+  </si>
+  <si>
+    <t>milky bar</t>
+  </si>
+  <si>
+    <t>cheese</t>
+  </si>
+  <si>
+    <t>licorice</t>
+  </si>
+  <si>
+    <t>chocolate bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,8 +195,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,21 +498,528 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="72.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>8.4</v>
+      </c>
+      <c r="C2" s="3">
+        <v>43611</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2.15</v>
+      </c>
+      <c r="C3" s="3">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>4.3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>3.5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1.67</v>
+      </c>
+      <c r="C8" s="3">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>3.44</v>
+      </c>
+      <c r="C9" s="3">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>2.39</v>
+      </c>
+      <c r="C11" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0.9</v>
+      </c>
+      <c r="C13" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>3.69</v>
+      </c>
+      <c r="C14" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>2.5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>10.99</v>
+      </c>
+      <c r="C17" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C19" s="3">
+        <v>43610</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>6.65</v>
+      </c>
+      <c r="C20" s="3">
+        <v>43610</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>6.44</v>
+      </c>
+      <c r="C21" s="3">
+        <v>43610</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="C22" s="3">
+        <v>43610</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3">
+        <v>43610</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>4.2</v>
+      </c>
+      <c r="C24" s="3">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>3.79</v>
+      </c>
+      <c r="C25" s="3">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C26" s="3">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1.69</v>
+      </c>
+      <c r="C27" s="3">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>10.7</v>
+      </c>
+      <c r="C29" s="3">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30" s="3">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" s="3">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32" s="3">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>17</v>
+      </c>
+      <c r="C33" s="5">
+        <v>43605</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>3.4</v>
+      </c>
+      <c r="C34" s="5">
+        <v>43605</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>3.4</v>
+      </c>
+      <c r="C35" s="5">
+        <v>43605</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36" s="5">
+        <v>43605</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" s="5">
+        <v>43605</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>8.1</v>
+      </c>
+      <c r="C38" s="5">
+        <v>43605</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>3.9</v>
+      </c>
+      <c r="C39" s="5">
+        <v>43605</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>2.35</v>
+      </c>
+      <c r="C40" s="5">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>1.69</v>
+      </c>
+      <c r="C41" s="5">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>7</v>
+      </c>
+      <c r="C42" s="5">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43">
+        <v>8.1</v>
+      </c>
+      <c r="C43" s="5">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44" s="5">
+        <v>43607</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <v>1.6</v>
+      </c>
+      <c r="C45" s="5">
+        <v>43607</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>8.4</v>
+      </c>
+      <c r="C46" s="5">
+        <v>43611</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Classified some of june's transactions. Changed look of some plots with different alpha values and plot heights.
</commit_message>
<xml_diff>
--- a/SpendTracker_ShinyApp/pastTransactionsData/manuallyEnteredGroceryReceipts.xlsx
+++ b/SpendTracker_ShinyApp/pastTransactionsData/manuallyEnteredGroceryReceipts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
   <si>
     <t>item</t>
   </si>
@@ -145,6 +145,117 @@
   </si>
   <si>
     <t>chocolate bar</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Nappies</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Laundry liquid</t>
+  </si>
+  <si>
+    <t>Only organic lasagne</t>
+  </si>
+  <si>
+    <t>Bathroom bags</t>
+  </si>
+  <si>
+    <t>Free range chicken</t>
+  </si>
+  <si>
+    <t>Only organic blueberry rice cakes</t>
+  </si>
+  <si>
+    <t>Moisturiser</t>
+  </si>
+  <si>
+    <t>Reusable bag</t>
+  </si>
+  <si>
+    <t>Popsicles</t>
+  </si>
+  <si>
+    <t>Apple juice</t>
+  </si>
+  <si>
+    <t>Soup</t>
+  </si>
+  <si>
+    <t>Tomatoes</t>
+  </si>
+  <si>
+    <t>Tomato paste</t>
+  </si>
+  <si>
+    <t>Red onions</t>
+  </si>
+  <si>
+    <t>Garlic</t>
+  </si>
+  <si>
+    <t>Free range eggs</t>
+  </si>
+  <si>
+    <t>lentils</t>
+  </si>
+  <si>
+    <t>Turtle beans</t>
+  </si>
+  <si>
+    <t>Kidney beans</t>
+  </si>
+  <si>
+    <t>Paprika</t>
+  </si>
+  <si>
+    <t>Whole peppercorns</t>
+  </si>
+  <si>
+    <t>Anchor cheese</t>
+  </si>
+  <si>
+    <t>Hairspray</t>
+  </si>
+  <si>
+    <t>Peanut butter</t>
+  </si>
+  <si>
+    <t>Brown onions</t>
+  </si>
+  <si>
+    <t>kumara</t>
+  </si>
+  <si>
+    <t>Pita bread</t>
+  </si>
+  <si>
+    <t>Avalanche coffee</t>
+  </si>
+  <si>
+    <t>Banana porridge</t>
+  </si>
+  <si>
+    <t>Only organic apple and cinnamon biscotti</t>
+  </si>
+  <si>
+    <t>Licorice allsorts</t>
+  </si>
+  <si>
+    <t>Only organic blueberry rice cake</t>
+  </si>
+  <si>
+    <t>Panadol</t>
+  </si>
+  <si>
+    <t>Dental floss</t>
+  </si>
+  <si>
+    <t>Corn chips</t>
   </si>
 </sst>
 </file>
@@ -498,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1015,6 +1126,611 @@
       </c>
       <c r="C46" s="5">
         <v>43611</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="4">
+        <v>8.4</v>
+      </c>
+      <c r="C47" s="3">
+        <v>43628</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48">
+        <v>5.3</v>
+      </c>
+      <c r="C48" s="3">
+        <v>43627</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49">
+        <v>15</v>
+      </c>
+      <c r="C49" s="3">
+        <v>43627</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50">
+        <v>3.41</v>
+      </c>
+      <c r="C50" s="3">
+        <v>43627</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51">
+        <v>3.41</v>
+      </c>
+      <c r="C51" s="3">
+        <v>43627</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52">
+        <v>7.99</v>
+      </c>
+      <c r="C52" s="3">
+        <v>43627</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53">
+        <v>5.4</v>
+      </c>
+      <c r="C53" s="3">
+        <v>43627</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54">
+        <v>3.6</v>
+      </c>
+      <c r="C54" s="3">
+        <v>43627</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55">
+        <v>7.99</v>
+      </c>
+      <c r="C55" s="3">
+        <v>43627</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56">
+        <v>2.99</v>
+      </c>
+      <c r="C56" s="3">
+        <v>43627</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57">
+        <v>4.2</v>
+      </c>
+      <c r="C57" s="3">
+        <v>43626</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58">
+        <v>36</v>
+      </c>
+      <c r="C58" s="3">
+        <v>43626</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59">
+        <v>7</v>
+      </c>
+      <c r="C59" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C61" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>4.3</v>
+      </c>
+      <c r="C62" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63">
+        <v>10</v>
+      </c>
+      <c r="C63" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B64">
+        <v>1.7</v>
+      </c>
+      <c r="C64" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B65">
+        <v>4.5</v>
+      </c>
+      <c r="C65" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B66">
+        <v>1.4</v>
+      </c>
+      <c r="C66" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67">
+        <v>4.5</v>
+      </c>
+      <c r="C67" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B68">
+        <v>2.7</v>
+      </c>
+      <c r="C68" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69">
+        <v>4</v>
+      </c>
+      <c r="C69" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70">
+        <v>7</v>
+      </c>
+      <c r="C70" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71">
+        <v>7.9</v>
+      </c>
+      <c r="C71" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72">
+        <v>6.7</v>
+      </c>
+      <c r="C72" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73">
+        <v>8.9</v>
+      </c>
+      <c r="C73" s="3">
+        <v>43625</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74">
+        <v>6.82</v>
+      </c>
+      <c r="C74" s="3">
+        <v>43624</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B75">
+        <v>7.25</v>
+      </c>
+      <c r="C75" s="3">
+        <v>43624</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76">
+        <v>6.65</v>
+      </c>
+      <c r="C76" s="3">
+        <v>43624</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B77">
+        <v>3.06</v>
+      </c>
+      <c r="C77" s="3">
+        <v>43624</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B78">
+        <v>3.37</v>
+      </c>
+      <c r="C78" s="3">
+        <v>43624</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" s="4">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C79" s="3">
+        <v>43623</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80">
+        <v>9.5</v>
+      </c>
+      <c r="C80" s="3">
+        <v>43623</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B81">
+        <v>9</v>
+      </c>
+      <c r="C81" s="3">
+        <v>43623</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B82">
+        <v>10</v>
+      </c>
+      <c r="C82" s="3">
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B83">
+        <v>4.2</v>
+      </c>
+      <c r="C83" s="3">
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84">
+        <v>4.49</v>
+      </c>
+      <c r="C84" s="3">
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B85">
+        <v>4.49</v>
+      </c>
+      <c r="C85" s="3">
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B86">
+        <v>6</v>
+      </c>
+      <c r="C86" s="3">
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B87">
+        <v>9</v>
+      </c>
+      <c r="C87" s="3">
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B88">
+        <v>5.98</v>
+      </c>
+      <c r="C88" s="3">
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="C89" s="3">
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B90">
+        <v>1.81</v>
+      </c>
+      <c r="C90" s="3">
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B91">
+        <v>8.4</v>
+      </c>
+      <c r="C91" s="3">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B92">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C92" s="3">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B93">
+        <v>6</v>
+      </c>
+      <c r="C93" s="3">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B94">
+        <v>3</v>
+      </c>
+      <c r="C94" s="3">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B95">
+        <v>4</v>
+      </c>
+      <c r="C95" s="3">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B96">
+        <v>4.5</v>
+      </c>
+      <c r="C96" s="3">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B97">
+        <v>4</v>
+      </c>
+      <c r="C97" s="3">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B98">
+        <v>3.69</v>
+      </c>
+      <c r="C98" s="3">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B99">
+        <v>4</v>
+      </c>
+      <c r="C99" s="3">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B100">
+        <v>3.5</v>
+      </c>
+      <c r="C100" s="3">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B101">
+        <v>3.6</v>
+      </c>
+      <c r="C101" s="3">
+        <v>43619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added June data plus a few minor tweaks.
</commit_message>
<xml_diff>
--- a/SpendTracker_ShinyApp/pastTransactionsData/manuallyEnteredGroceryReceipts.xlsx
+++ b/SpendTracker_ShinyApp/pastTransactionsData/manuallyEnteredGroceryReceipts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
   <si>
     <t>item</t>
   </si>
@@ -256,6 +256,81 @@
   </si>
   <si>
     <t>Corn chips</t>
+  </si>
+  <si>
+    <t>Peeled tomatoes</t>
+  </si>
+  <si>
+    <t>Ginger</t>
+  </si>
+  <si>
+    <t>Toothpaste</t>
+  </si>
+  <si>
+    <t>Flowers</t>
+  </si>
+  <si>
+    <t>Kiwi fruit</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Spring onions</t>
+  </si>
+  <si>
+    <t>Yoghurt</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Only organic breakfast</t>
+  </si>
+  <si>
+    <t>Baby wipes</t>
+  </si>
+  <si>
+    <t>Sweet potato</t>
+  </si>
+  <si>
+    <t>Vegemite</t>
+  </si>
+  <si>
+    <t>Hand sanitiser</t>
+  </si>
+  <si>
+    <t>Only organic beef pasta</t>
+  </si>
+  <si>
+    <t>Only organic cheese pasta</t>
+  </si>
+  <si>
+    <t>Pumpkin</t>
+  </si>
+  <si>
+    <t>Bananas</t>
+  </si>
+  <si>
+    <t>Only organic rice cakes</t>
+  </si>
+  <si>
+    <t>Courgette</t>
+  </si>
+  <si>
+    <t>Mandarins</t>
+  </si>
+  <si>
+    <t>toffee</t>
+  </si>
+  <si>
+    <t>Kiwi garden yoghurt drops</t>
+  </si>
+  <si>
+    <t>Band-Aid adhesive strips</t>
+  </si>
+  <si>
+    <t>Licorice</t>
   </si>
 </sst>
 </file>
@@ -609,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,6 +695,7 @@
     <col min="1" max="1" width="72.140625" customWidth="1"/>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1731,6 +1807,535 @@
       </c>
       <c r="C101" s="3">
         <v>43619</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B102">
+        <v>5.6</v>
+      </c>
+      <c r="C102" s="3">
+        <v>43646</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B103">
+        <v>4.5</v>
+      </c>
+      <c r="C103" s="3">
+        <v>43646</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B104">
+        <v>0.9</v>
+      </c>
+      <c r="C104" s="3">
+        <v>43646</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B105">
+        <v>1.7</v>
+      </c>
+      <c r="C105" s="3">
+        <v>43646</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B106">
+        <v>9.99</v>
+      </c>
+      <c r="C106" s="3">
+        <v>43646</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B107">
+        <v>2.5</v>
+      </c>
+      <c r="C107" s="3">
+        <v>43646</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B108">
+        <v>2.9</v>
+      </c>
+      <c r="C108" s="3">
+        <v>43645</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B109">
+        <v>1.7</v>
+      </c>
+      <c r="C109" s="3">
+        <v>43645</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B110">
+        <v>1.4</v>
+      </c>
+      <c r="C110" s="3">
+        <v>43645</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B111">
+        <v>1.3</v>
+      </c>
+      <c r="C111" s="3">
+        <v>43645</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B112">
+        <v>7.5</v>
+      </c>
+      <c r="C112" s="3">
+        <v>43645</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B113">
+        <v>2.8</v>
+      </c>
+      <c r="C113" s="3">
+        <v>43645</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B114">
+        <v>3.4</v>
+      </c>
+      <c r="C114" s="3">
+        <v>43643</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B115">
+        <v>3.4</v>
+      </c>
+      <c r="C115" s="3">
+        <v>43643</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B116">
+        <v>8.4</v>
+      </c>
+      <c r="C116" s="3">
+        <v>43643</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B117">
+        <v>12</v>
+      </c>
+      <c r="C117" s="3">
+        <v>43643</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B118">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C118" s="3">
+        <v>43643</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B119">
+        <v>8.4</v>
+      </c>
+      <c r="C119" s="3">
+        <v>43643</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B120">
+        <v>5.3</v>
+      </c>
+      <c r="C120" s="3">
+        <v>43642</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B121">
+        <v>3</v>
+      </c>
+      <c r="C121" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B122">
+        <v>6</v>
+      </c>
+      <c r="C122" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B123">
+        <v>13</v>
+      </c>
+      <c r="C123" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B124">
+        <v>8.5</v>
+      </c>
+      <c r="C124" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B125">
+        <v>10</v>
+      </c>
+      <c r="C125" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B126">
+        <v>3.5</v>
+      </c>
+      <c r="C126" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B127">
+        <v>3.5</v>
+      </c>
+      <c r="C127" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B128">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C128" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B129">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C129" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B130">
+        <v>3</v>
+      </c>
+      <c r="C130" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B131">
+        <v>0.3</v>
+      </c>
+      <c r="C131" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B132">
+        <v>3.5</v>
+      </c>
+      <c r="C132" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B133">
+        <v>4.3</v>
+      </c>
+      <c r="C133" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B134">
+        <v>1.4</v>
+      </c>
+      <c r="C134" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B135">
+        <v>1.7</v>
+      </c>
+      <c r="C135" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B136">
+        <v>7.6</v>
+      </c>
+      <c r="C136" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B137">
+        <v>1.6</v>
+      </c>
+      <c r="C137" s="3">
+        <v>43639</v>
+      </c>
+      <c r="D137" s="3"/>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B138">
+        <v>3</v>
+      </c>
+      <c r="C138" s="3">
+        <v>43639</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B139">
+        <v>2</v>
+      </c>
+      <c r="C139" s="3">
+        <v>43639</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B140">
+        <v>3.4</v>
+      </c>
+      <c r="C140" s="3">
+        <v>43632</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B141">
+        <v>3.4</v>
+      </c>
+      <c r="C141" s="3">
+        <v>43632</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B142">
+        <v>4</v>
+      </c>
+      <c r="C142" s="3">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B143">
+        <v>6</v>
+      </c>
+      <c r="C143" s="3">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B144">
+        <v>5.7</v>
+      </c>
+      <c r="C144" s="3">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B145">
+        <v>2.25</v>
+      </c>
+      <c r="C145" s="3">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B146">
+        <v>1.2</v>
+      </c>
+      <c r="C146" s="3">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B147">
+        <v>4.2</v>
+      </c>
+      <c r="C147" s="3">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B148">
+        <v>4</v>
+      </c>
+      <c r="C148" s="3">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B149" s="4">
+        <v>1</v>
+      </c>
+      <c r="C149" s="3">
+        <v>43634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>